<commit_message>
Remove unneeded uC datasheet and update part tracking excel for 1.2 planned parts
</commit_message>
<xml_diff>
--- a/doc/node-doc/part_tracking_light_valve_node.xlsx
+++ b/doc/node-doc/part_tracking_light_valve_node.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianteam/Developer/light-valves/doc/node-doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40204F36-F9CC-C74F-9BC4-6BAFB2137857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B5EA4B-5BED-9743-91B8-3B8DF645A8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21120" xr2:uid="{E64AAD0A-1366-0840-8175-817CEFEBBF59}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <t>Part</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>NCP718ASN500T1G</t>
+  </si>
+  <si>
+    <t>cheaper / smaller rect</t>
+  </si>
+  <si>
+    <t>BAV199S</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/filter/diodes-rectifiers-arrays/286?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIALAAxwDMdIh1cFtVIAuoQA4AuUIAMq8ATgEsAdgHMQAX0JwA7BGggUkDDgLEy4AExg4ADj2ce-SENGSZ8kAFpTq9aICu2kpHIBWRiAQcsnYwiCBiACYC9mBUEOYCfrwAnty4AujYKEFAA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/panjit-international-inc/BAV199S-R1-00001/14661140</t>
   </si>
 </sst>
 </file>
@@ -211,8 +223,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -228,7 +240,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -527,7 +539,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,8 +711,17 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>

</xml_diff>